<commit_message>
Further refactoring in PlayerActor. Created RandomPlayerActor.
</commit_message>
<xml_diff>
--- a/games.Shithead/doc/Messages order.xlsx
+++ b/games.Shithead/doc/Messages order.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\tournament\games.Shithead\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{E681C7F9-4F1E-4F15-B933-741A3A77AEF7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="4035" xr2:uid="{E681C7F9-4F1E-4F15-B933-741A3A77AEF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>Message</t>
   </si>
@@ -57,9 +53,6 @@
   </si>
   <si>
     <t>PublicDealMessage</t>
-  </si>
-  <si>
-    <t>PlayersOrderMessage</t>
   </si>
   <si>
     <t>PlayerActionInfo</t>
@@ -452,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D45D006-E4CB-4E1C-8D9A-41A32A933797}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.140625" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -539,29 +532,29 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -572,32 +565,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-    </row>
+    <row r="14" spans="1:3" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>